<commit_message>
Solved 126 and Trees
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aryan\Work\DSA &amp; CP\DSA 450 Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C6A743-4920-4A1B-B73A-48B3031A48EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA53788-7267-4C81-B53F-CE9E9CF6AB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1929,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3755,7 +3755,7 @@
       <c r="C139" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D139" s="13" t="s">
+      <c r="D139" s="14" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved: 166 167 168
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aryan\Work\DSA &amp; CP\DSA 450 Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34942AC4-3AC4-46BF-8B26-B6F679E39D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7C3CAC-0976-40DC-8421-62EF6E2F6A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -564,12 +564,6 @@
     <t>Mirror of a tree</t>
   </si>
   <si>
-    <t>Inorder Traversal of a tree both using recursion and Iteration</t>
-  </si>
-  <si>
-    <t>Preorder Traversal of a tree both using recursion and Iteration</t>
-  </si>
-  <si>
     <t>Postorder Traversal of a tree both using recursion and Iteration</t>
   </si>
   <si>
@@ -1429,13 +1423,45 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Inorder Traversal of a tree both using recursion and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Iteration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Preorder Traversal of a tree both using recursion and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Iteration</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1508,6 +1534,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1941,8 +1975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C186" sqref="C186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1964,7 +1998,7 @@
     </row>
     <row r="4" spans="1:5" ht="21">
       <c r="A4" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -4118,7 +4152,7 @@
         <v>160</v>
       </c>
       <c r="D164" s="14" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">
@@ -4215,7 +4249,7 @@
       <c r="C171" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D171" s="13" t="s">
+      <c r="D171" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4229,7 +4263,7 @@
       <c r="C172" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D172" s="13" t="s">
+      <c r="D172" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4275,7 +4309,7 @@
       <c r="C177" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D177" s="13" t="s">
+      <c r="D177" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4289,7 +4323,7 @@
       <c r="C178" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D178" s="13" t="s">
+      <c r="D178" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4303,7 +4337,7 @@
       <c r="C179" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D179" s="13" t="s">
+      <c r="D179" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4317,7 +4351,7 @@
       <c r="C180" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D180" s="13" t="s">
+      <c r="D180" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4331,7 +4365,7 @@
       <c r="C181" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D181" s="13" t="s">
+      <c r="D181" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4343,9 +4377,9 @@
         <v>171</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D182" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="D182" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4357,9 +4391,9 @@
         <v>171</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D183" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="D183" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4371,7 +4405,7 @@
         <v>171</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D184" s="13" t="s">
         <v>4</v>
@@ -4385,7 +4419,7 @@
         <v>171</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D185" s="13" t="s">
         <v>4</v>
@@ -4399,7 +4433,7 @@
         <v>171</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D186" s="13" t="s">
         <v>4</v>
@@ -4413,7 +4447,7 @@
         <v>171</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D187" s="13" t="s">
         <v>4</v>
@@ -4427,7 +4461,7 @@
         <v>171</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D188" s="13" t="s">
         <v>4</v>
@@ -4441,7 +4475,7 @@
         <v>171</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D189" s="13" t="s">
         <v>4</v>
@@ -4455,7 +4489,7 @@
         <v>171</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D190" s="13" t="s">
         <v>4</v>
@@ -4469,7 +4503,7 @@
         <v>171</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D191" s="13" t="s">
         <v>4</v>
@@ -4483,7 +4517,7 @@
         <v>171</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D192" s="13" t="s">
         <v>4</v>
@@ -4497,7 +4531,7 @@
         <v>171</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D193" s="13" t="s">
         <v>4</v>
@@ -4511,7 +4545,7 @@
         <v>171</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D194" s="13" t="s">
         <v>4</v>
@@ -4525,7 +4559,7 @@
         <v>171</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D195" s="13" t="s">
         <v>4</v>
@@ -4539,7 +4573,7 @@
         <v>171</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D196" s="13" t="s">
         <v>4</v>
@@ -4553,7 +4587,7 @@
         <v>171</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D197" s="13" t="s">
         <v>4</v>
@@ -4567,7 +4601,7 @@
         <v>171</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D198" s="13" t="s">
         <v>4</v>
@@ -4581,7 +4615,7 @@
         <v>171</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D199" s="13" t="s">
         <v>4</v>
@@ -4595,7 +4629,7 @@
         <v>171</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D200" s="13" t="s">
         <v>4</v>
@@ -4609,7 +4643,7 @@
         <v>171</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D201" s="13" t="s">
         <v>4</v>
@@ -4623,7 +4657,7 @@
         <v>171</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D202" s="13" t="s">
         <v>4</v>
@@ -4637,7 +4671,7 @@
         <v>171</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D203" s="13" t="s">
         <v>4</v>
@@ -4651,7 +4685,7 @@
         <v>171</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D204" s="13" t="s">
         <v>4</v>
@@ -4665,7 +4699,7 @@
         <v>171</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D205" s="13" t="s">
         <v>4</v>
@@ -4679,7 +4713,7 @@
         <v>171</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D206" s="13" t="s">
         <v>4</v>
@@ -4693,7 +4727,7 @@
         <v>171</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D207" s="13" t="s">
         <v>4</v>
@@ -4707,7 +4741,7 @@
         <v>171</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D208" s="13" t="s">
         <v>4</v>
@@ -4721,7 +4755,7 @@
         <v>171</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D209" s="13" t="s">
         <v>4</v>
@@ -4735,7 +4769,7 @@
         <v>171</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D210" s="13" t="s">
         <v>4</v>
@@ -4749,7 +4783,7 @@
         <v>171</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D211" s="13" t="s">
         <v>4</v>
@@ -4770,10 +4804,10 @@
         <v>197</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>4</v>
@@ -4784,10 +4818,10 @@
         <v>198</v>
       </c>
       <c r="B215" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C215" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="C215" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>4</v>
@@ -4798,10 +4832,10 @@
         <v>199</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D216" s="13" t="s">
         <v>4</v>
@@ -4812,10 +4846,10 @@
         <v>200</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D217" s="13" t="s">
         <v>4</v>
@@ -4826,10 +4860,10 @@
         <v>201</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>4</v>
@@ -4840,10 +4874,10 @@
         <v>202</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>4</v>
@@ -4854,10 +4888,10 @@
         <v>203</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C220" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D220" s="13" t="s">
         <v>4</v>
@@ -4868,10 +4902,10 @@
         <v>204</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D221" s="13" t="s">
         <v>4</v>
@@ -4882,10 +4916,10 @@
         <v>205</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D222" s="13" t="s">
         <v>4</v>
@@ -4896,10 +4930,10 @@
         <v>206</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D223" s="13" t="s">
         <v>4</v>
@@ -4910,10 +4944,10 @@
         <v>207</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D224" s="13" t="s">
         <v>4</v>
@@ -4924,10 +4958,10 @@
         <v>208</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D225" s="13" t="s">
         <v>4</v>
@@ -4938,10 +4972,10 @@
         <v>209</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D226" s="13" t="s">
         <v>4</v>
@@ -4952,10 +4986,10 @@
         <v>210</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D227" s="13" t="s">
         <v>4</v>
@@ -4966,10 +5000,10 @@
         <v>211</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D228" s="13" t="s">
         <v>4</v>
@@ -4980,10 +5014,10 @@
         <v>212</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D229" s="13" t="s">
         <v>4</v>
@@ -4994,10 +5028,10 @@
         <v>213</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D230" s="13" t="s">
         <v>4</v>
@@ -5008,10 +5042,10 @@
         <v>214</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D231" s="13" t="s">
         <v>4</v>
@@ -5022,10 +5056,10 @@
         <v>215</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D232" s="13" t="s">
         <v>4</v>
@@ -5036,10 +5070,10 @@
         <v>216</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D233" s="13" t="s">
         <v>4</v>
@@ -5050,10 +5084,10 @@
         <v>217</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D234" s="13" t="s">
         <v>4</v>
@@ -5064,10 +5098,10 @@
         <v>218</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D235" s="13" t="s">
         <v>4</v>
@@ -5086,10 +5120,10 @@
         <v>219</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D238" s="13" t="s">
         <v>4</v>
@@ -5100,10 +5134,10 @@
         <v>220</v>
       </c>
       <c r="B239" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C239" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="C239" s="5" t="s">
-        <v>232</v>
       </c>
       <c r="D239" s="13" t="s">
         <v>4</v>
@@ -5114,10 +5148,10 @@
         <v>221</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D240" s="13" t="s">
         <v>4</v>
@@ -5128,10 +5162,10 @@
         <v>222</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D241" s="13" t="s">
         <v>4</v>
@@ -5142,10 +5176,10 @@
         <v>223</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D242" s="13" t="s">
         <v>4</v>
@@ -5156,10 +5190,10 @@
         <v>224</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D243" s="13" t="s">
         <v>4</v>
@@ -5170,10 +5204,10 @@
         <v>225</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D244" s="13" t="s">
         <v>4</v>
@@ -5184,10 +5218,10 @@
         <v>226</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D245" s="13" t="s">
         <v>4</v>
@@ -5198,10 +5232,10 @@
         <v>227</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D246" s="13" t="s">
         <v>4</v>
@@ -5212,10 +5246,10 @@
         <v>228</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D247" s="13" t="s">
         <v>4</v>
@@ -5226,10 +5260,10 @@
         <v>229</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C248" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D248" s="13" t="s">
         <v>4</v>
@@ -5240,10 +5274,10 @@
         <v>230</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D249" s="13" t="s">
         <v>4</v>
@@ -5254,10 +5288,10 @@
         <v>231</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D250" s="13" t="s">
         <v>4</v>
@@ -5268,10 +5302,10 @@
         <v>232</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C251" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D251" s="13" t="s">
         <v>4</v>
@@ -5282,10 +5316,10 @@
         <v>233</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C252" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D252" s="13" t="s">
         <v>4</v>
@@ -5296,10 +5330,10 @@
         <v>234</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C253" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D253" s="13" t="s">
         <v>4</v>
@@ -5310,10 +5344,10 @@
         <v>235</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D254" s="13" t="s">
         <v>4</v>
@@ -5324,10 +5358,10 @@
         <v>236</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C255" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D255" s="13" t="s">
         <v>4</v>
@@ -5338,10 +5372,10 @@
         <v>237</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C256" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D256" s="13" t="s">
         <v>4</v>
@@ -5352,10 +5386,10 @@
         <v>238</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C257" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D257" s="13" t="s">
         <v>4</v>
@@ -5366,10 +5400,10 @@
         <v>239</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D258" s="13" t="s">
         <v>4</v>
@@ -5380,10 +5414,10 @@
         <v>240</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D259" s="13" t="s">
         <v>4</v>
@@ -5394,10 +5428,10 @@
         <v>241</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D260" s="13" t="s">
         <v>4</v>
@@ -5408,10 +5442,10 @@
         <v>242</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D261" s="13" t="s">
         <v>4</v>
@@ -5422,10 +5456,10 @@
         <v>243</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D262" s="13" t="s">
         <v>4</v>
@@ -5436,10 +5470,10 @@
         <v>244</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D263" s="13" t="s">
         <v>4</v>
@@ -5450,10 +5484,10 @@
         <v>245</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D264" s="13" t="s">
         <v>4</v>
@@ -5464,10 +5498,10 @@
         <v>246</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D265" s="13" t="s">
         <v>4</v>
@@ -5478,10 +5512,10 @@
         <v>247</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D266" s="13" t="s">
         <v>4</v>
@@ -5492,10 +5526,10 @@
         <v>248</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C267" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D267" s="13" t="s">
         <v>4</v>
@@ -5506,10 +5540,10 @@
         <v>249</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C268" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D268" s="13" t="s">
         <v>4</v>
@@ -5520,10 +5554,10 @@
         <v>250</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C269" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D269" s="13" t="s">
         <v>4</v>
@@ -5534,10 +5568,10 @@
         <v>251</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C270" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D270" s="13" t="s">
         <v>4</v>
@@ -5548,7 +5582,7 @@
         <v>252</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C271" s="5" t="s">
         <v>87</v>
@@ -5562,10 +5596,10 @@
         <v>253</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D272" s="13" t="s">
         <v>4</v>
@@ -5584,10 +5618,10 @@
         <v>254</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D275" s="13" t="s">
         <v>4</v>
@@ -5598,10 +5632,10 @@
         <v>255</v>
       </c>
       <c r="B276" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C276" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="C276" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="D276" s="13" t="s">
         <v>4</v>
@@ -5612,10 +5646,10 @@
         <v>256</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D277" s="13" t="s">
         <v>4</v>
@@ -5626,10 +5660,10 @@
         <v>257</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D278" s="13" t="s">
         <v>4</v>
@@ -5640,10 +5674,10 @@
         <v>258</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C279" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D279" s="13" t="s">
         <v>4</v>
@@ -5654,10 +5688,10 @@
         <v>259</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D280" s="13" t="s">
         <v>4</v>
@@ -5668,10 +5702,10 @@
         <v>260</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D281" s="13" t="s">
         <v>4</v>
@@ -5682,10 +5716,10 @@
         <v>261</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D282" s="13" t="s">
         <v>4</v>
@@ -5696,10 +5730,10 @@
         <v>262</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D283" s="13" t="s">
         <v>4</v>
@@ -5710,10 +5744,10 @@
         <v>263</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C284" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D284" s="13" t="s">
         <v>4</v>
@@ -5724,10 +5758,10 @@
         <v>264</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C285" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D285" s="13" t="s">
         <v>4</v>
@@ -5738,10 +5772,10 @@
         <v>265</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D286" s="13" t="s">
         <v>4</v>
@@ -5752,10 +5786,10 @@
         <v>266</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C287" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D287" s="13" t="s">
         <v>4</v>
@@ -5766,10 +5800,10 @@
         <v>267</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D288" s="13" t="s">
         <v>4</v>
@@ -5780,10 +5814,10 @@
         <v>268</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D289" s="13" t="s">
         <v>4</v>
@@ -5794,10 +5828,10 @@
         <v>269</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C290" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D290" s="13" t="s">
         <v>4</v>
@@ -5808,10 +5842,10 @@
         <v>270</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D291" s="13" t="s">
         <v>4</v>
@@ -5822,10 +5856,10 @@
         <v>271</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D292" s="13" t="s">
         <v>4</v>
@@ -5836,10 +5870,10 @@
         <v>272</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D293" s="13" t="s">
         <v>4</v>
@@ -5858,10 +5892,10 @@
         <v>273</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C296" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D296" s="13" t="s">
         <v>4</v>
@@ -5872,10 +5906,10 @@
         <v>274</v>
       </c>
       <c r="B297" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C297" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="C297" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="D297" s="13" t="s">
         <v>4</v>
@@ -5886,10 +5920,10 @@
         <v>275</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D298" s="13" t="s">
         <v>4</v>
@@ -5900,10 +5934,10 @@
         <v>276</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D299" s="13" t="s">
         <v>4</v>
@@ -5914,10 +5948,10 @@
         <v>277</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D300" s="13" t="s">
         <v>4</v>
@@ -5928,10 +5962,10 @@
         <v>278</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C301" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D301" s="13" t="s">
         <v>4</v>
@@ -5942,10 +5976,10 @@
         <v>279</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D302" s="13" t="s">
         <v>4</v>
@@ -5956,10 +5990,10 @@
         <v>280</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C303" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D303" s="13" t="s">
         <v>4</v>
@@ -5970,10 +6004,10 @@
         <v>281</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D304" s="13" t="s">
         <v>4</v>
@@ -5984,10 +6018,10 @@
         <v>282</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D305" s="13" t="s">
         <v>4</v>
@@ -5998,10 +6032,10 @@
         <v>283</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D306" s="13" t="s">
         <v>4</v>
@@ -6012,10 +6046,10 @@
         <v>284</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C307" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D307" s="13" t="s">
         <v>4</v>
@@ -6026,10 +6060,10 @@
         <v>285</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C308" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D308" s="13" t="s">
         <v>4</v>
@@ -6040,10 +6074,10 @@
         <v>286</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C309" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D309" s="13" t="s">
         <v>4</v>
@@ -6054,10 +6088,10 @@
         <v>287</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C310" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D310" s="13" t="s">
         <v>4</v>
@@ -6068,10 +6102,10 @@
         <v>288</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D311" s="13" t="s">
         <v>4</v>
@@ -6082,10 +6116,10 @@
         <v>289</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C312" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D312" s="13" t="s">
         <v>4</v>
@@ -6096,10 +6130,10 @@
         <v>290</v>
       </c>
       <c r="B313" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C313" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D313" s="13" t="s">
         <v>4</v>
@@ -6110,10 +6144,10 @@
         <v>291</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C314" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D314" s="13" t="s">
         <v>4</v>
@@ -6124,10 +6158,10 @@
         <v>292</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D315" s="13" t="s">
         <v>4</v>
@@ -6138,10 +6172,10 @@
         <v>293</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D316" s="13" t="s">
         <v>4</v>
@@ -6152,10 +6186,10 @@
         <v>294</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C317" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D317" s="13" t="s">
         <v>4</v>
@@ -6166,10 +6200,10 @@
         <v>295</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C318" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D318" s="13" t="s">
         <v>4</v>
@@ -6180,10 +6214,10 @@
         <v>296</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C319" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D319" s="13" t="s">
         <v>4</v>
@@ -6194,10 +6228,10 @@
         <v>297</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C320" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D320" s="13" t="s">
         <v>4</v>
@@ -6208,10 +6242,10 @@
         <v>298</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C321" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D321" s="13" t="s">
         <v>4</v>
@@ -6222,10 +6256,10 @@
         <v>299</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C322" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D322" s="13" t="s">
         <v>4</v>
@@ -6236,10 +6270,10 @@
         <v>300</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C323" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D323" s="13" t="s">
         <v>4</v>
@@ -6250,10 +6284,10 @@
         <v>301</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C324" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D324" s="13" t="s">
         <v>4</v>
@@ -6264,10 +6298,10 @@
         <v>302</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C325" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D325" s="13" t="s">
         <v>4</v>
@@ -6278,10 +6312,10 @@
         <v>303</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C326" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D326" s="13" t="s">
         <v>4</v>
@@ -6292,10 +6326,10 @@
         <v>304</v>
       </c>
       <c r="B327" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C327" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D327" s="13" t="s">
         <v>4</v>
@@ -6306,10 +6340,10 @@
         <v>305</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C328" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D328" s="13" t="s">
         <v>4</v>
@@ -6320,10 +6354,10 @@
         <v>306</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C329" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D329" s="13" t="s">
         <v>4</v>
@@ -6334,10 +6368,10 @@
         <v>307</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C330" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D330" s="13" t="s">
         <v>4</v>
@@ -6348,10 +6382,10 @@
         <v>308</v>
       </c>
       <c r="B331" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C331" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D331" s="13" t="s">
         <v>4</v>
@@ -6362,10 +6396,10 @@
         <v>309</v>
       </c>
       <c r="B332" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C332" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D332" s="13" t="s">
         <v>4</v>
@@ -6376,10 +6410,10 @@
         <v>310</v>
       </c>
       <c r="B333" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C333" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D333" s="13" t="s">
         <v>4</v>
@@ -6398,10 +6432,10 @@
         <v>311</v>
       </c>
       <c r="B336" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C336" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D336" s="13" t="s">
         <v>4</v>
@@ -6412,10 +6446,10 @@
         <v>312</v>
       </c>
       <c r="B337" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C337" s="5" t="s">
         <v>324</v>
-      </c>
-      <c r="C337" s="5" t="s">
-        <v>326</v>
       </c>
       <c r="D337" s="13" t="s">
         <v>4</v>
@@ -6426,10 +6460,10 @@
         <v>313</v>
       </c>
       <c r="B338" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C338" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D338" s="13" t="s">
         <v>4</v>
@@ -6440,10 +6474,10 @@
         <v>314</v>
       </c>
       <c r="B339" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C339" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D339" s="13" t="s">
         <v>4</v>
@@ -6454,10 +6488,10 @@
         <v>315</v>
       </c>
       <c r="B340" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C340" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D340" s="13" t="s">
         <v>4</v>
@@ -6468,10 +6502,10 @@
         <v>316</v>
       </c>
       <c r="B341" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C341" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D341" s="13" t="s">
         <v>4</v>
@@ -6482,10 +6516,10 @@
         <v>317</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C342" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D342" s="13" t="s">
         <v>4</v>
@@ -6496,10 +6530,10 @@
         <v>318</v>
       </c>
       <c r="B343" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C343" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D343" s="13" t="s">
         <v>4</v>
@@ -6510,10 +6544,10 @@
         <v>319</v>
       </c>
       <c r="B344" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C344" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D344" s="13" t="s">
         <v>4</v>
@@ -6524,10 +6558,10 @@
         <v>320</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C345" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D345" s="13" t="s">
         <v>4</v>
@@ -6538,10 +6572,10 @@
         <v>321</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C346" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D346" s="13" t="s">
         <v>4</v>
@@ -6552,10 +6586,10 @@
         <v>322</v>
       </c>
       <c r="B347" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C347" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D347" s="13" t="s">
         <v>4</v>
@@ -6566,10 +6600,10 @@
         <v>323</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C348" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D348" s="13" t="s">
         <v>4</v>
@@ -6580,10 +6614,10 @@
         <v>324</v>
       </c>
       <c r="B349" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C349" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D349" s="13" t="s">
         <v>4</v>
@@ -6594,10 +6628,10 @@
         <v>325</v>
       </c>
       <c r="B350" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C350" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D350" s="13" t="s">
         <v>4</v>
@@ -6608,10 +6642,10 @@
         <v>326</v>
       </c>
       <c r="B351" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C351" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D351" s="13" t="s">
         <v>4</v>
@@ -6622,10 +6656,10 @@
         <v>327</v>
       </c>
       <c r="B352" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C352" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D352" s="13" t="s">
         <v>4</v>
@@ -6636,10 +6670,10 @@
         <v>328</v>
       </c>
       <c r="B353" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C353" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D353" s="13" t="s">
         <v>4</v>
@@ -6658,10 +6692,10 @@
         <v>329</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C356" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D356" s="13" t="s">
         <v>4</v>
@@ -6672,10 +6706,10 @@
         <v>330</v>
       </c>
       <c r="B357" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C357" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="C357" s="5" t="s">
-        <v>345</v>
       </c>
       <c r="D357" s="13" t="s">
         <v>4</v>
@@ -6686,10 +6720,10 @@
         <v>331</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C358" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D358" s="13" t="s">
         <v>4</v>
@@ -6700,10 +6734,10 @@
         <v>332</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C359" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D359" s="13" t="s">
         <v>4</v>
@@ -6714,10 +6748,10 @@
         <v>333</v>
       </c>
       <c r="B360" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C360" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D360" s="13" t="s">
         <v>4</v>
@@ -6728,10 +6762,10 @@
         <v>334</v>
       </c>
       <c r="B361" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C361" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D361" s="13" t="s">
         <v>4</v>
@@ -6742,10 +6776,10 @@
         <v>335</v>
       </c>
       <c r="B362" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C362" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D362" s="13" t="s">
         <v>4</v>
@@ -6756,10 +6790,10 @@
         <v>336</v>
       </c>
       <c r="B363" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C363" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D363" s="13" t="s">
         <v>4</v>
@@ -6770,10 +6804,10 @@
         <v>337</v>
       </c>
       <c r="B364" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C364" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D364" s="13" t="s">
         <v>4</v>
@@ -6784,10 +6818,10 @@
         <v>338</v>
       </c>
       <c r="B365" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C365" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D365" s="13" t="s">
         <v>4</v>
@@ -6798,10 +6832,10 @@
         <v>339</v>
       </c>
       <c r="B366" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C366" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D366" s="13" t="s">
         <v>4</v>
@@ -6812,10 +6846,10 @@
         <v>340</v>
       </c>
       <c r="B367" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C367" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D367" s="13" t="s">
         <v>4</v>
@@ -6826,10 +6860,10 @@
         <v>341</v>
       </c>
       <c r="B368" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C368" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D368" s="13" t="s">
         <v>4</v>
@@ -6840,10 +6874,10 @@
         <v>342</v>
       </c>
       <c r="B369" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C369" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D369" s="13" t="s">
         <v>4</v>
@@ -6854,10 +6888,10 @@
         <v>343</v>
       </c>
       <c r="B370" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C370" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D370" s="13" t="s">
         <v>4</v>
@@ -6868,10 +6902,10 @@
         <v>344</v>
       </c>
       <c r="B371" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C371" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D371" s="13" t="s">
         <v>4</v>
@@ -6882,10 +6916,10 @@
         <v>345</v>
       </c>
       <c r="B372" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C372" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D372" s="13" t="s">
         <v>4</v>
@@ -6896,10 +6930,10 @@
         <v>346</v>
       </c>
       <c r="B373" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C373" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D373" s="13" t="s">
         <v>4</v>
@@ -6910,10 +6944,10 @@
         <v>347</v>
       </c>
       <c r="B374" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C374" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D374" s="13" t="s">
         <v>4</v>
@@ -6924,10 +6958,10 @@
         <v>348</v>
       </c>
       <c r="B375" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C375" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D375" s="13" t="s">
         <v>4</v>
@@ -6938,10 +6972,10 @@
         <v>349</v>
       </c>
       <c r="B376" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C376" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D376" s="13" t="s">
         <v>4</v>
@@ -6952,10 +6986,10 @@
         <v>350</v>
       </c>
       <c r="B377" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C377" s="5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D377" s="13" t="s">
         <v>4</v>
@@ -6966,10 +7000,10 @@
         <v>351</v>
       </c>
       <c r="B378" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C378" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D378" s="13" t="s">
         <v>4</v>
@@ -6980,10 +7014,10 @@
         <v>352</v>
       </c>
       <c r="B379" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C379" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D379" s="13" t="s">
         <v>4</v>
@@ -6994,10 +7028,10 @@
         <v>353</v>
       </c>
       <c r="B380" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C380" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D380" s="13" t="s">
         <v>4</v>
@@ -7008,10 +7042,10 @@
         <v>354</v>
       </c>
       <c r="B381" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C381" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D381" s="13" t="s">
         <v>4</v>
@@ -7022,10 +7056,10 @@
         <v>355</v>
       </c>
       <c r="B382" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C382" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D382" s="13" t="s">
         <v>4</v>
@@ -7036,10 +7070,10 @@
         <v>356</v>
       </c>
       <c r="B383" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C383" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D383" s="13" t="s">
         <v>4</v>
@@ -7050,10 +7084,10 @@
         <v>357</v>
       </c>
       <c r="B384" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C384" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D384" s="13" t="s">
         <v>4</v>
@@ -7064,10 +7098,10 @@
         <v>358</v>
       </c>
       <c r="B385" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C385" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D385" s="13" t="s">
         <v>4</v>
@@ -7078,10 +7112,10 @@
         <v>359</v>
       </c>
       <c r="B386" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C386" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D386" s="13" t="s">
         <v>4</v>
@@ -7092,10 +7126,10 @@
         <v>360</v>
       </c>
       <c r="B387" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C387" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D387" s="13" t="s">
         <v>4</v>
@@ -7106,10 +7140,10 @@
         <v>361</v>
       </c>
       <c r="B388" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C388" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D388" s="13" t="s">
         <v>4</v>
@@ -7120,10 +7154,10 @@
         <v>362</v>
       </c>
       <c r="B389" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C389" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D389" s="13" t="s">
         <v>4</v>
@@ -7134,10 +7168,10 @@
         <v>363</v>
       </c>
       <c r="B390" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C390" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D390" s="13" t="s">
         <v>4</v>
@@ -7148,10 +7182,10 @@
         <v>364</v>
       </c>
       <c r="B391" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C391" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D391" s="13" t="s">
         <v>4</v>
@@ -7162,10 +7196,10 @@
         <v>365</v>
       </c>
       <c r="B392" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C392" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D392" s="13" t="s">
         <v>4</v>
@@ -7176,10 +7210,10 @@
         <v>366</v>
       </c>
       <c r="B393" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C393" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D393" s="13" t="s">
         <v>4</v>
@@ -7190,10 +7224,10 @@
         <v>367</v>
       </c>
       <c r="B394" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C394" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D394" s="13" t="s">
         <v>4</v>
@@ -7204,10 +7238,10 @@
         <v>368</v>
       </c>
       <c r="B395" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C395" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D395" s="13" t="s">
         <v>4</v>
@@ -7218,10 +7252,10 @@
         <v>369</v>
       </c>
       <c r="B396" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C396" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D396" s="13" t="s">
         <v>4</v>
@@ -7232,10 +7266,10 @@
         <v>370</v>
       </c>
       <c r="B397" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C397" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D397" s="13" t="s">
         <v>4</v>
@@ -7246,10 +7280,10 @@
         <v>371</v>
       </c>
       <c r="B398" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C398" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D398" s="13" t="s">
         <v>4</v>
@@ -7260,10 +7294,10 @@
         <v>372</v>
       </c>
       <c r="B399" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C399" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D399" s="13" t="s">
         <v>4</v>
@@ -7282,10 +7316,10 @@
         <v>373</v>
       </c>
       <c r="B402" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C402" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D402" s="13" t="s">
         <v>4</v>
@@ -7296,10 +7330,10 @@
         <v>374</v>
       </c>
       <c r="B403" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C403" s="5" t="s">
         <v>387</v>
-      </c>
-      <c r="C403" s="5" t="s">
-        <v>389</v>
       </c>
       <c r="D403" s="13" t="s">
         <v>4</v>
@@ -7310,10 +7344,10 @@
         <v>375</v>
       </c>
       <c r="B404" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C404" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D404" s="13" t="s">
         <v>4</v>
@@ -7324,7 +7358,7 @@
         <v>376</v>
       </c>
       <c r="B405" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C405" s="5" t="s">
         <v>89</v>
@@ -7338,10 +7372,10 @@
         <v>377</v>
       </c>
       <c r="B406" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C406" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D406" s="13" t="s">
         <v>4</v>
@@ -7352,10 +7386,10 @@
         <v>378</v>
       </c>
       <c r="B407" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C407" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D407" s="13" t="s">
         <v>4</v>
@@ -7374,10 +7408,10 @@
         <v>379</v>
       </c>
       <c r="B410" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C410" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D410" s="13" t="s">
         <v>4</v>
@@ -7388,10 +7422,10 @@
         <v>380</v>
       </c>
       <c r="B411" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C411" s="5" t="s">
         <v>393</v>
-      </c>
-      <c r="C411" s="5" t="s">
-        <v>395</v>
       </c>
       <c r="D411" s="13" t="s">
         <v>4</v>
@@ -7402,10 +7436,10 @@
         <v>381</v>
       </c>
       <c r="B412" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C412" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D412" s="13" t="s">
         <v>4</v>
@@ -7416,10 +7450,10 @@
         <v>382</v>
       </c>
       <c r="B413" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C413" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D413" s="13" t="s">
         <v>4</v>
@@ -7430,10 +7464,10 @@
         <v>383</v>
       </c>
       <c r="B414" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C414" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D414" s="13" t="s">
         <v>4</v>
@@ -7444,10 +7478,10 @@
         <v>384</v>
       </c>
       <c r="B415" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C415" s="5" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D415" s="13" t="s">
         <v>4</v>
@@ -7458,10 +7492,10 @@
         <v>385</v>
       </c>
       <c r="B416" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C416" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D416" s="13" t="s">
         <v>4</v>
@@ -7472,10 +7506,10 @@
         <v>386</v>
       </c>
       <c r="B417" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C417" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D417" s="13" t="s">
         <v>4</v>
@@ -7486,10 +7520,10 @@
         <v>387</v>
       </c>
       <c r="B418" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C418" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D418" s="13" t="s">
         <v>4</v>
@@ -7500,10 +7534,10 @@
         <v>388</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C419" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D419" s="13" t="s">
         <v>4</v>
@@ -7514,10 +7548,10 @@
         <v>389</v>
       </c>
       <c r="B420" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C420" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D420" s="13" t="s">
         <v>4</v>
@@ -7528,10 +7562,10 @@
         <v>390</v>
       </c>
       <c r="B421" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C421" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D421" s="13" t="s">
         <v>4</v>
@@ -7542,10 +7576,10 @@
         <v>391</v>
       </c>
       <c r="B422" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C422" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D422" s="13" t="s">
         <v>4</v>
@@ -7556,10 +7590,10 @@
         <v>392</v>
       </c>
       <c r="B423" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C423" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D423" s="13" t="s">
         <v>4</v>
@@ -7570,10 +7604,10 @@
         <v>393</v>
       </c>
       <c r="B424" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C424" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D424" s="13" t="s">
         <v>4</v>
@@ -7584,10 +7618,10 @@
         <v>394</v>
       </c>
       <c r="B425" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C425" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D425" s="13" t="s">
         <v>4</v>
@@ -7598,10 +7632,10 @@
         <v>395</v>
       </c>
       <c r="B426" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C426" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D426" s="13" t="s">
         <v>4</v>
@@ -7612,10 +7646,10 @@
         <v>396</v>
       </c>
       <c r="B427" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C427" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D427" s="13" t="s">
         <v>4</v>
@@ -7626,10 +7660,10 @@
         <v>397</v>
       </c>
       <c r="B428" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C428" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D428" s="13" t="s">
         <v>4</v>
@@ -7640,10 +7674,10 @@
         <v>398</v>
       </c>
       <c r="B429" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C429" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D429" s="13" t="s">
         <v>4</v>
@@ -7654,10 +7688,10 @@
         <v>399</v>
       </c>
       <c r="B430" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C430" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D430" s="13" t="s">
         <v>4</v>
@@ -7668,10 +7702,10 @@
         <v>400</v>
       </c>
       <c r="B431" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C431" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D431" s="13" t="s">
         <v>4</v>
@@ -7682,10 +7716,10 @@
         <v>401</v>
       </c>
       <c r="B432" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C432" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D432" s="13" t="s">
         <v>4</v>
@@ -7696,10 +7730,10 @@
         <v>402</v>
       </c>
       <c r="B433" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C433" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D433" s="13" t="s">
         <v>4</v>
@@ -7710,10 +7744,10 @@
         <v>403</v>
       </c>
       <c r="B434" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C434" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D434" s="13" t="s">
         <v>4</v>
@@ -7724,10 +7758,10 @@
         <v>404</v>
       </c>
       <c r="B435" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C435" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D435" s="13" t="s">
         <v>4</v>
@@ -7738,10 +7772,10 @@
         <v>405</v>
       </c>
       <c r="B436" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C436" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D436" s="13" t="s">
         <v>4</v>
@@ -7752,10 +7786,10 @@
         <v>406</v>
       </c>
       <c r="B437" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C437" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D437" s="13" t="s">
         <v>4</v>
@@ -7766,10 +7800,10 @@
         <v>407</v>
       </c>
       <c r="B438" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C438" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D438" s="13" t="s">
         <v>4</v>
@@ -7780,10 +7814,10 @@
         <v>408</v>
       </c>
       <c r="B439" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C439" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D439" s="13" t="s">
         <v>4</v>
@@ -7794,10 +7828,10 @@
         <v>409</v>
       </c>
       <c r="B440" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C440" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D440" s="13" t="s">
         <v>4</v>
@@ -7808,10 +7842,10 @@
         <v>410</v>
       </c>
       <c r="B441" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C441" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D441" s="13" t="s">
         <v>4</v>
@@ -7822,10 +7856,10 @@
         <v>411</v>
       </c>
       <c r="B442" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C442" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D442" s="13" t="s">
         <v>4</v>
@@ -7836,10 +7870,10 @@
         <v>412</v>
       </c>
       <c r="B443" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C443" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D443" s="13" t="s">
         <v>4</v>
@@ -7850,10 +7884,10 @@
         <v>413</v>
       </c>
       <c r="B444" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C444" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D444" s="13" t="s">
         <v>4</v>
@@ -7864,10 +7898,10 @@
         <v>414</v>
       </c>
       <c r="B445" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C445" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D445" s="13" t="s">
         <v>4</v>
@@ -7878,10 +7912,10 @@
         <v>415</v>
       </c>
       <c r="B446" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C446" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D446" s="13" t="s">
         <v>4</v>
@@ -7892,10 +7926,10 @@
         <v>416</v>
       </c>
       <c r="B447" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C447" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D447" s="13" t="s">
         <v>4</v>
@@ -7906,10 +7940,10 @@
         <v>417</v>
       </c>
       <c r="B448" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C448" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D448" s="13" t="s">
         <v>4</v>
@@ -7920,10 +7954,10 @@
         <v>418</v>
       </c>
       <c r="B449" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C449" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D449" s="13" t="s">
         <v>4</v>
@@ -7934,10 +7968,10 @@
         <v>419</v>
       </c>
       <c r="B450" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C450" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D450" s="13" t="s">
         <v>4</v>
@@ -7948,10 +7982,10 @@
         <v>420</v>
       </c>
       <c r="B451" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C451" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D451" s="13" t="s">
         <v>4</v>
@@ -7962,10 +7996,10 @@
         <v>421</v>
       </c>
       <c r="B452" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C452" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D452" s="13" t="s">
         <v>4</v>
@@ -7976,10 +8010,10 @@
         <v>422</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C453" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D453" s="13" t="s">
         <v>4</v>
@@ -7990,10 +8024,10 @@
         <v>423</v>
       </c>
       <c r="B454" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C454" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D454" s="13" t="s">
         <v>4</v>
@@ -8004,10 +8038,10 @@
         <v>424</v>
       </c>
       <c r="B455" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C455" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D455" s="13" t="s">
         <v>4</v>
@@ -8018,10 +8052,10 @@
         <v>425</v>
       </c>
       <c r="B456" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C456" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D456" s="13" t="s">
         <v>4</v>
@@ -8032,10 +8066,10 @@
         <v>426</v>
       </c>
       <c r="B457" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C457" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D457" s="13" t="s">
         <v>4</v>
@@ -8046,10 +8080,10 @@
         <v>427</v>
       </c>
       <c r="B458" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C458" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D458" s="13" t="s">
         <v>4</v>
@@ -8060,10 +8094,10 @@
         <v>428</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C459" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D459" s="13" t="s">
         <v>4</v>
@@ -8074,10 +8108,10 @@
         <v>429</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C460" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D460" s="13" t="s">
         <v>4</v>
@@ -8088,10 +8122,10 @@
         <v>430</v>
       </c>
       <c r="B461" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C461" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D461" s="13" t="s">
         <v>4</v>
@@ -8102,10 +8136,10 @@
         <v>431</v>
       </c>
       <c r="B462" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C462" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D462" s="13" t="s">
         <v>4</v>
@@ -8116,10 +8150,10 @@
         <v>432</v>
       </c>
       <c r="B463" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C463" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D463" s="13" t="s">
         <v>4</v>
@@ -8130,10 +8164,10 @@
         <v>433</v>
       </c>
       <c r="B464" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C464" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D464" s="13" t="s">
         <v>4</v>
@@ -8144,10 +8178,10 @@
         <v>434</v>
       </c>
       <c r="B465" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C465" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D465" s="13" t="s">
         <v>4</v>
@@ -8158,10 +8192,10 @@
         <v>435</v>
       </c>
       <c r="B466" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C466" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D466" s="13" t="s">
         <v>4</v>
@@ -8172,10 +8206,10 @@
         <v>436</v>
       </c>
       <c r="B467" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C467" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D467" s="13" t="s">
         <v>4</v>
@@ -8186,10 +8220,10 @@
         <v>437</v>
       </c>
       <c r="B468" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C468" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D468" s="13" t="s">
         <v>4</v>
@@ -8200,10 +8234,10 @@
         <v>438</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C469" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D469" s="13" t="s">
         <v>4</v>
@@ -8223,10 +8257,10 @@
         <v>439</v>
       </c>
       <c r="B472" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C472" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D472" s="13" t="s">
         <v>4</v>
@@ -8237,10 +8271,10 @@
         <v>440</v>
       </c>
       <c r="B473" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C473" s="5" t="s">
         <v>453</v>
-      </c>
-      <c r="C473" s="5" t="s">
-        <v>455</v>
       </c>
       <c r="D473" s="13" t="s">
         <v>4</v>
@@ -8251,10 +8285,10 @@
         <v>441</v>
       </c>
       <c r="B474" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C474" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D474" s="13" t="s">
         <v>4</v>
@@ -8265,10 +8299,10 @@
         <v>442</v>
       </c>
       <c r="B475" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C475" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D475" s="13" t="s">
         <v>4</v>
@@ -8279,10 +8313,10 @@
         <v>443</v>
       </c>
       <c r="B476" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C476" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D476" s="13" t="s">
         <v>4</v>
@@ -8293,10 +8327,10 @@
         <v>444</v>
       </c>
       <c r="B477" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C477" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D477" s="13" t="s">
         <v>4</v>
@@ -8307,10 +8341,10 @@
         <v>445</v>
       </c>
       <c r="B478" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C478" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D478" s="13" t="s">
         <v>4</v>
@@ -8321,10 +8355,10 @@
         <v>446</v>
       </c>
       <c r="B479" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C479" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D479" s="13" t="s">
         <v>4</v>
@@ -8335,10 +8369,10 @@
         <v>447</v>
       </c>
       <c r="B480" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C480" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D480" s="13" t="s">
         <v>4</v>
@@ -8349,10 +8383,10 @@
         <v>448</v>
       </c>
       <c r="B481" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C481" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D481" s="13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Solved: LC5 LC14 LC9 LC 226 LC513
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1917,11 +1917,11 @@
   </sheetPr>
   <dimension ref="A1:E494"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A438" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C455" activeCellId="0" sqref="C455"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.45703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.5"/>
@@ -8067,7 +8067,7 @@
       <c r="C462" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="D462" s="9" t="s">
+      <c r="D462" s="24" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>